<commit_message>
Update Excel with new issue #7
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,33 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>[FEATURE REQUEST] &lt;title&gt;dfsdfsdfsdf</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-03-21T09:12:12Z</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>enhancement</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #8
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,6 +502,33 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>[BUG] deployment failing</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-03-24T08:21:23Z</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #9
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,33 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>[BUG] deployment failing</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-03-24T08:23:49Z</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #10
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,33 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>[BUG] ghdwedgweyd</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-03-24T08:32:16Z</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #11
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,6 +583,33 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Resource newrelic_synthetics_monitor: Cannot unset validation_string</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-03-24T09:02:25Z</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #12
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,6 +610,33 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>newrelic_alert_channel Resource newrelic_synthetics_monitor: Cannot unset validation_string</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-03-24T09:04:06Z</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #13
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -637,6 +637,33 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>newrelic_alert_channel</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-03-24T09:05:44Z</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #14
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,6 +664,33 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>dfdddg. newrelic_alert_channel dfdfdfdf</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-03-24T09:11:58Z</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>enhancement</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #15
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,6 +691,33 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>I am using newrelic alert putting rule which is failing</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-03-24T09:14:38Z</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #16
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -718,6 +718,33 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>newrelic_alert_condition and newrelic_cloud_aws_integrations</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-03-24T10:26:30Z</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #17
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +745,33 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>FR_OPERATIONS issue</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-03-25T11:47:03Z</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #18
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,6 +772,33 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>hjasgdjahgsdhjags</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-03-25T11:48:19Z</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #19
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -799,6 +799,33 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FR_OPERATIONS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:37:01Z</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #20
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -826,6 +826,33 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FR_HIRING</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:40:25Z</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #21
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -853,6 +853,33 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>FR_HIRING</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:41:40Z</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>enhancement</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #22
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -880,6 +880,33 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>jhasgcdahjsgdhajsgdhas</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:42:33Z</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #23
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -907,6 +907,33 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FR_SALES</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:54:29Z</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #24
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -934,6 +934,33 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>[BUG] &lt;title&gt;ahjkdahjsd</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:55:02Z</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #25
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -961,6 +961,33 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>[BUG] &lt;title&gt;sdasda</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:56:53Z</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #26
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -988,6 +988,33 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>[FEATURE REQUEST] &lt;title&gt;</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:58:51Z</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>enhancement</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #27
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1015,6 +1015,33 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>[FEATURE REQUEST] &lt;title&gt;</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-03-26T06:59:28Z</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>enhancement</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #28
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1042,6 +1042,33 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>[BUG] &lt;title&gt;</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-03-26T07:00:05Z</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel with new issue #29
</commit_message>
<xml_diff>
--- a/issues.xlsx
+++ b/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1069,6 +1069,33 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>[BUG] &lt;title&gt;</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-03-26T07:00:42Z</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>bug</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>